<commit_message>
Remove hash dependency, make group names in data_hash characters
</commit_message>
<xml_diff>
--- a/helper/Eikon.xlsx
+++ b/helper/Eikon.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\Users\Fernando.Cantu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\Users\Nour.Barnat\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -159,72 +159,70 @@
   <volType type="realTimeData">
     <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 09:28:16</v>
+        <v>Updated at 15:49:55</v>
         <stp/>
-        <stp>{EEAE09C6-455F-4AE7-B52A-FE7495AA9904}_x0000_</stp>
+        <stp>{7D59DA56-78E0-43BE-B037-1B4E6D3820CF}_x0000_</stp>
         <tr r="AK3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:24:34</v>
+        <v>Updated at 15:49:55</v>
         <stp/>
-        <stp>{08F59E99-0289-438C-AFB5-3F4938BDEEF8}_x0000_</stp>
+        <stp>{33652F3D-757A-4128-8E24-78506F9973FF}_x0000_</stp>
+        <tr r="AC3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:49:55</v>
+        <stp/>
+        <stp>{68FBE21B-905B-4B08-BA66-85E85C344697}_x0000_</stp>
         <tr r="Y3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:54</v>
         <stp/>
-        <stp>{84405A58-DA55-4913-834B-ECCB7080814C}_x0000_</stp>
+        <stp>{F7CB99FF-4688-4D00-A212-CE123B571E77}_x0000_</stp>
+        <tr r="AG3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:49:46</v>
+        <stp/>
+        <stp>{EFEAD925-8B02-4EB9-BAD5-2D35A2767AC7}_x0000_</stp>
+        <tr r="U3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:49:46</v>
+        <stp/>
+        <stp>{A3A06510-F2CE-4316-B524-AB5268861E0E}_x0000_</stp>
         <tr r="M3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:32:02</v>
+        <v>Updated at 15:49:46</v>
         <stp/>
-        <stp>{82FF288D-5EDE-4B3A-9361-13BCAB1C3452}_x0000_</stp>
-        <tr r="AO3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:24:33</v>
-        <stp/>
-        <stp>{E082D2D3-EAB0-4942-ABCF-135FA257353A}_x0000_</stp>
+        <stp>{BB4AABB1-B655-446E-BA74-A56EF9814915}_x0000_</stp>
         <tr r="Q3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:45</v>
         <stp/>
-        <stp>{E09AD1B9-B2C4-4C66-B760-A7E0A0529FB2}_x0000_</stp>
+        <stp>{26036738-6393-480F-9432-6D955FFC0FE7}_x0000_</stp>
         <tr r="I3" s="2"/>
       </tp>
-    </main>
-    <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:50:02</v>
         <stp/>
-        <stp>{A897A5ED-4342-4E63-89AD-EC3B3A547E29}_x0000_</stp>
+        <stp>{CB71FF21-2C18-4BC9-8AF1-16B2DF2F796B}_x0000_</stp>
+        <tr r="A3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:49:55</v>
+        <stp/>
+        <stp>{88EEBE18-F634-4F1A-A9BC-09398101D5D8}_x0000_</stp>
         <tr r="E3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:46</v>
         <stp/>
-        <stp>{426907F7-DFC5-4572-8E99-D0D1112BC1CB}_x0000_</stp>
-        <tr r="AC3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:24:35</v>
-        <stp/>
-        <stp>{6571444F-F433-4CFE-A961-7668511C37FF}_x0000_</stp>
-        <tr r="A3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:24:34</v>
-        <stp/>
-        <stp>{5B86E031-6B3B-41FC-A68F-5EDD5CCB2309}_x0000_</stp>
-        <tr r="U3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:24:34</v>
-        <stp/>
-        <stp>{56E0054C-21B3-4E2B-A413-6CAEE4621579}_x0000_</stp>
-        <tr r="AG3" s="2"/>
+        <stp>{91EB106C-90CD-453A-9B64-734F8B05498F}_x0000_</stp>
+        <tr r="AO3" s="2"/>
       </tp>
     </main>
   </volType>
@@ -531,9 +529,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A199" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ226" sqref="AQ226"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -614,47 +612,47 @@
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>_xll.RHistory(C2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",B4)</f>
-        <v>Updated at 09:24:35</v>
+        <v>Updated at 15:50:02</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.RHistory(G2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",F4)</f>
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:55</v>
       </c>
       <c r="I3" t="str">
         <f>_xll.RHistory(K2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",J4)</f>
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:45</v>
       </c>
       <c r="M3" t="str">
         <f>_xll.RHistory(O2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",N4)</f>
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:46</v>
       </c>
       <c r="Q3" t="str">
         <f>_xll.RHistory(S2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",R4)</f>
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:46</v>
       </c>
       <c r="U3" t="str">
         <f>_xll.RHistory(W2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",V4)</f>
-        <v>Updated at 09:24:34</v>
+        <v>Updated at 15:49:46</v>
       </c>
       <c r="Y3" t="str">
         <f>_xll.RHistory(AA2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",Z4)</f>
-        <v>Updated at 09:24:34</v>
+        <v>Updated at 15:49:55</v>
       </c>
       <c r="AC3" t="str">
         <f>_xll.RHistory(AE2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AD4)</f>
-        <v>Updated at 09:24:33</v>
+        <v>Updated at 15:49:55</v>
       </c>
       <c r="AG3" t="str">
         <f>_xll.RHistory(AI2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AH4)</f>
-        <v>Updated at 09:24:34</v>
+        <v>Updated at 15:49:54</v>
       </c>
       <c r="AK3" t="str">
         <f>_xll.RHistory(AM2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AL4)</f>
-        <v>Updated at 09:28:16</v>
+        <v>Updated at 15:49:55</v>
       </c>
       <c r="AO3" t="str">
         <f>_xll.RHistory(AQ2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AP4)</f>
-        <v>Updated at 09:32:02</v>
+        <v>Updated at 15:49:46</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
@@ -5204,7 +5202,7 @@
         <v>44012</v>
       </c>
       <c r="AM70">
-        <v>17021.88</v>
+        <v>17062.45</v>
       </c>
       <c r="AP70" s="2">
         <v>39263</v>
@@ -5272,7 +5270,7 @@
         <v>44043</v>
       </c>
       <c r="AM71">
-        <v>16898.349999999999</v>
+        <v>18217.330000000002</v>
       </c>
       <c r="AP71" s="2">
         <v>39294</v>
@@ -5336,6 +5334,12 @@
       <c r="AI72">
         <v>1225820</v>
       </c>
+      <c r="AL72" s="2">
+        <v>44074</v>
+      </c>
+      <c r="AM72">
+        <v>16737.97</v>
+      </c>
       <c r="AP72" s="2">
         <v>39325</v>
       </c>
@@ -14470,6 +14474,12 @@
       <c r="AE226">
         <v>54.4</v>
       </c>
+      <c r="AH226" s="2">
+        <v>44012</v>
+      </c>
+      <c r="AI226">
+        <v>0</v>
+      </c>
       <c r="AP226" s="2">
         <v>44012</v>
       </c>
@@ -14482,13 +14492,31 @@
         <v>44043</v>
       </c>
       <c r="O227">
-        <v>1594</v>
+        <v>1350</v>
       </c>
       <c r="R227" s="2">
         <v>44043</v>
       </c>
       <c r="S227">
-        <v>463</v>
+        <v>522</v>
+      </c>
+      <c r="V227" s="2">
+        <v>44043</v>
+      </c>
+      <c r="W227">
+        <v>54.2</v>
+      </c>
+      <c r="Z227" s="2">
+        <v>44043</v>
+      </c>
+      <c r="AA227">
+        <v>58.1</v>
+      </c>
+      <c r="AD227" s="2">
+        <v>44043</v>
+      </c>
+      <c r="AE227">
+        <v>54.2</v>
       </c>
       <c r="AP227" s="2">
         <v>44043</v>
@@ -14498,6 +14526,12 @@
       </c>
     </row>
     <row r="228" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="N228" s="2">
+        <v>44074</v>
+      </c>
+      <c r="O228">
+        <v>1475</v>
+      </c>
       <c r="AP228" s="2">
         <v>44074</v>
       </c>

</xml_diff>

<commit_message>
Update catalog to have new variables for nowcast
</commit_message>
<xml_diff>
--- a/helper/Eikon.xlsx
+++ b/helper/Eikon.xlsx
@@ -159,70 +159,70 @@
   <volType type="realTimeData">
     <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
         <stp/>
-        <stp>{7D59DA56-78E0-43BE-B037-1B4E6D3820CF}_x0000_</stp>
+        <stp>{22446A75-6580-49D0-A5C7-EACEE9802E12}_x0000_</stp>
+        <tr r="E3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{6D9B80F3-934F-48EE-ADEB-8572FFC6E848}_x0000_</stp>
+        <tr r="M3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{61D24252-C389-4F55-BA45-CD9258DC1AEE}_x0000_</stp>
+        <tr r="Y3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{A3B55305-80C2-4660-8E2E-2D0C3DD639E0}_x0000_</stp>
+        <tr r="AG3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{3B2E30B3-A0E5-4DA2-A9D6-6572FE4A8290}_x0000_</stp>
+        <tr r="Q3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{EEC4506D-05E2-48B3-9395-397ACC0456A3}_x0000_</stp>
+        <tr r="U3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:04</v>
+        <stp/>
+        <stp>{FFC918F4-00C0-4C52-91F2-274825BC9B11}_x0000_</stp>
+        <tr r="I3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:05</v>
+        <stp/>
+        <stp>{81E97F22-8C65-480C-85BC-5745287FFCD7}_x0000_</stp>
+        <tr r="AO3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 09:26:04</v>
+        <stp/>
+        <stp>{CDEC0E0D-AEFE-4312-9D4F-3AB226FCD39C}_x0000_</stp>
         <tr r="AK3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
         <stp/>
-        <stp>{33652F3D-757A-4128-8E24-78506F9973FF}_x0000_</stp>
+        <stp>{A34ED1E5-C454-4312-9236-F51CDCDDAB13}_x0000_</stp>
         <tr r="AC3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
         <stp/>
-        <stp>{68FBE21B-905B-4B08-BA66-85E85C344697}_x0000_</stp>
-        <tr r="Y3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:54</v>
-        <stp/>
-        <stp>{F7CB99FF-4688-4D00-A212-CE123B571E77}_x0000_</stp>
-        <tr r="AG3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:46</v>
-        <stp/>
-        <stp>{EFEAD925-8B02-4EB9-BAD5-2D35A2767AC7}_x0000_</stp>
-        <tr r="U3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:46</v>
-        <stp/>
-        <stp>{A3A06510-F2CE-4316-B524-AB5268861E0E}_x0000_</stp>
-        <tr r="M3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:46</v>
-        <stp/>
-        <stp>{BB4AABB1-B655-446E-BA74-A56EF9814915}_x0000_</stp>
-        <tr r="Q3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:45</v>
-        <stp/>
-        <stp>{26036738-6393-480F-9432-6D955FFC0FE7}_x0000_</stp>
-        <tr r="I3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:50:02</v>
-        <stp/>
-        <stp>{CB71FF21-2C18-4BC9-8AF1-16B2DF2F796B}_x0000_</stp>
+        <stp>{0A9CA1AB-86FB-4001-9623-589C8C0415CB}_x0000_</stp>
         <tr r="A3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:55</v>
-        <stp/>
-        <stp>{88EEBE18-F634-4F1A-A9BC-09398101D5D8}_x0000_</stp>
-        <tr r="E3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 15:49:46</v>
-        <stp/>
-        <stp>{91EB106C-90CD-453A-9B64-734F8B05498F}_x0000_</stp>
-        <tr r="AO3" s="2"/>
       </tp>
     </main>
   </volType>
@@ -530,7 +530,7 @@
   <dimension ref="A1:AQ244"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
@@ -612,47 +612,47 @@
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>_xll.RHistory(C2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",B4)</f>
-        <v>Updated at 15:50:02</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.RHistory(G2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",F4)</f>
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="I3" t="str">
         <f>_xll.RHistory(K2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",J4)</f>
-        <v>Updated at 15:49:45</v>
+        <v>Updated at 09:26:04</v>
       </c>
       <c r="M3" t="str">
         <f>_xll.RHistory(O2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",N4)</f>
-        <v>Updated at 15:49:46</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="Q3" t="str">
         <f>_xll.RHistory(S2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",R4)</f>
-        <v>Updated at 15:49:46</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="U3" t="str">
         <f>_xll.RHistory(W2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",V4)</f>
-        <v>Updated at 15:49:46</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="Y3" t="str">
         <f>_xll.RHistory(AA2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",Z4)</f>
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="AC3" t="str">
         <f>_xll.RHistory(AE2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AD4)</f>
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="AG3" t="str">
         <f>_xll.RHistory(AI2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AH4)</f>
-        <v>Updated at 15:49:54</v>
+        <v>Updated at 09:26:05</v>
       </c>
       <c r="AK3" t="str">
         <f>_xll.RHistory(AM2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AL4)</f>
-        <v>Updated at 15:49:55</v>
+        <v>Updated at 09:26:04</v>
       </c>
       <c r="AO3" t="str">
         <f>_xll.RHistory(AQ2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AP4)</f>
-        <v>Updated at 15:49:46</v>
+        <v>Updated at 09:26:05</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
@@ -5134,7 +5134,7 @@
         <v>43982</v>
       </c>
       <c r="AM69">
-        <v>19057.11</v>
+        <v>19053.14</v>
       </c>
       <c r="AP69" s="2">
         <v>39233</v>
@@ -5202,7 +5202,7 @@
         <v>44012</v>
       </c>
       <c r="AM70">
-        <v>17062.45</v>
+        <v>16987.62</v>
       </c>
       <c r="AP70" s="2">
         <v>39263</v>
@@ -5270,7 +5270,7 @@
         <v>44043</v>
       </c>
       <c r="AM71">
-        <v>18217.330000000002</v>
+        <v>18367.54</v>
       </c>
       <c r="AP71" s="2">
         <v>39294</v>
@@ -5338,7 +5338,7 @@
         <v>44074</v>
       </c>
       <c r="AM72">
-        <v>16737.97</v>
+        <v>17942.7</v>
       </c>
       <c r="AP72" s="2">
         <v>39325</v>
@@ -10076,7 +10076,7 @@
         <v>43677</v>
       </c>
       <c r="K149">
-        <v>1332050000</v>
+        <v>1844340000</v>
       </c>
       <c r="N149" s="2">
         <v>41670</v>
@@ -10758,7 +10758,7 @@
         <v>44012</v>
       </c>
       <c r="K160">
-        <v>805860000</v>
+        <v>893180000</v>
       </c>
       <c r="N160" s="2">
         <v>42004</v>
@@ -10816,6 +10816,12 @@
       <c r="G161">
         <v>13923000000</v>
       </c>
+      <c r="J161" s="2">
+        <v>44043</v>
+      </c>
+      <c r="K161">
+        <v>2518600000</v>
+      </c>
       <c r="N161" s="2">
         <v>42035</v>
       </c>
@@ -14216,7 +14222,7 @@
         <v>43861</v>
       </c>
       <c r="AQ221">
-        <v>28.69</v>
+        <v>28.67</v>
       </c>
     </row>
     <row r="222" spans="2:43" x14ac:dyDescent="0.3">
@@ -14272,7 +14278,7 @@
         <v>43890</v>
       </c>
       <c r="AQ222">
-        <v>28.03</v>
+        <v>28.02</v>
       </c>
     </row>
     <row r="223" spans="2:43" x14ac:dyDescent="0.3">
@@ -14336,7 +14342,7 @@
         <v>43951</v>
       </c>
       <c r="C224">
-        <v>16322000000</v>
+        <v>20340000000</v>
       </c>
       <c r="F224" s="2">
         <v>43982</v>
@@ -14392,7 +14398,7 @@
         <v>43982</v>
       </c>
       <c r="C225">
-        <v>16168000000</v>
+        <v>20017000000</v>
       </c>
       <c r="F225" s="2">
         <v>44012</v>
@@ -14440,10 +14446,22 @@
         <v>43982</v>
       </c>
       <c r="AQ225">
-        <v>24.31</v>
+        <v>24.28</v>
       </c>
     </row>
     <row r="226" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B226" s="2">
+        <v>44012</v>
+      </c>
+      <c r="C226">
+        <v>24215000000</v>
+      </c>
+      <c r="F226" s="2">
+        <v>44043</v>
+      </c>
+      <c r="G226">
+        <v>9050000000</v>
+      </c>
       <c r="N226" s="2">
         <v>44012</v>
       </c>
@@ -14484,7 +14502,7 @@
         <v>44012</v>
       </c>
       <c r="AQ226">
-        <v>22.71</v>
+        <v>22.35</v>
       </c>
     </row>
     <row r="227" spans="2:43" x14ac:dyDescent="0.3">
@@ -14522,7 +14540,7 @@
         <v>44043</v>
       </c>
       <c r="AQ227">
-        <v>22.47</v>
+        <v>23.045000000000002</v>
       </c>
     </row>
     <row r="228" spans="2:43" x14ac:dyDescent="0.3">
@@ -14530,13 +14548,19 @@
         <v>44074</v>
       </c>
       <c r="O228">
-        <v>1475</v>
+        <v>1518</v>
+      </c>
+      <c r="R228" s="2">
+        <v>44074</v>
+      </c>
+      <c r="S228">
+        <v>597</v>
       </c>
       <c r="AP228" s="2">
         <v>44074</v>
       </c>
       <c r="AQ228">
-        <v>24.04</v>
+        <v>23.73</v>
       </c>
     </row>
     <row r="229" spans="2:43" x14ac:dyDescent="0.3">
@@ -14544,7 +14568,7 @@
         <v>44104</v>
       </c>
       <c r="AQ229">
-        <v>24.57</v>
+        <v>23.74</v>
       </c>
     </row>
     <row r="230" spans="2:43" x14ac:dyDescent="0.3">
@@ -14552,7 +14576,7 @@
         <v>44135</v>
       </c>
       <c r="AQ230">
-        <v>25.57</v>
+        <v>24.6</v>
       </c>
     </row>
     <row r="231" spans="2:43" x14ac:dyDescent="0.3">
@@ -14560,7 +14584,7 @@
         <v>44165</v>
       </c>
       <c r="AQ231">
-        <v>26.35</v>
+        <v>25.71</v>
       </c>
     </row>
     <row r="232" spans="2:43" x14ac:dyDescent="0.3">
@@ -14568,7 +14592,7 @@
         <v>44196</v>
       </c>
       <c r="AQ232">
-        <v>27.135000000000002</v>
+        <v>26.535</v>
       </c>
     </row>
     <row r="233" spans="2:43" x14ac:dyDescent="0.3">
@@ -14576,7 +14600,7 @@
         <v>44227</v>
       </c>
       <c r="AQ233">
-        <v>28.26</v>
+        <v>27.86</v>
       </c>
     </row>
     <row r="234" spans="2:43" x14ac:dyDescent="0.3">
@@ -14584,7 +14608,7 @@
         <v>44255</v>
       </c>
       <c r="AQ234">
-        <v>28.26</v>
+        <v>28.16</v>
       </c>
     </row>
     <row r="235" spans="2:43" x14ac:dyDescent="0.3">
@@ -14592,7 +14616,7 @@
         <v>44286</v>
       </c>
       <c r="AQ235">
-        <v>28.26</v>
+        <v>28.46</v>
       </c>
     </row>
     <row r="236" spans="2:43" x14ac:dyDescent="0.3">
@@ -14600,7 +14624,7 @@
         <v>44316</v>
       </c>
       <c r="AQ236">
-        <v>29.274999999999999</v>
+        <v>29.574999999999999</v>
       </c>
     </row>
     <row r="237" spans="2:43" x14ac:dyDescent="0.3">
@@ -14608,7 +14632,7 @@
         <v>44347</v>
       </c>
       <c r="AQ237">
-        <v>29.261825999999999</v>
+        <v>29.661826000000001</v>
       </c>
     </row>
     <row r="238" spans="2:43" x14ac:dyDescent="0.3">
@@ -14616,7 +14640,7 @@
         <v>44377</v>
       </c>
       <c r="AQ238">
-        <v>29.250485999999999</v>
+        <v>29.650486000000001</v>
       </c>
     </row>
     <row r="239" spans="2:43" x14ac:dyDescent="0.3">
@@ -14624,7 +14648,7 @@
         <v>44408</v>
       </c>
       <c r="AQ239">
-        <v>29.599146000000001</v>
+        <v>29.699145999999999</v>
       </c>
     </row>
     <row r="240" spans="2:43" x14ac:dyDescent="0.3">
@@ -14632,7 +14656,7 @@
         <v>44439</v>
       </c>
       <c r="AQ240">
-        <v>29.607806</v>
+        <v>29.707806000000001</v>
       </c>
     </row>
     <row r="241" spans="42:43" x14ac:dyDescent="0.3">
@@ -14640,7 +14664,7 @@
         <v>44469</v>
       </c>
       <c r="AQ241">
-        <v>29.616465000000002</v>
+        <v>29.716464999999999</v>
       </c>
     </row>
     <row r="242" spans="42:43" x14ac:dyDescent="0.3">
@@ -14648,7 +14672,7 @@
         <v>44500</v>
       </c>
       <c r="AQ242">
-        <v>29.635124999999999</v>
+        <v>29.725124999999998</v>
       </c>
     </row>
     <row r="243" spans="42:43" x14ac:dyDescent="0.3">
@@ -14656,7 +14680,7 @@
         <v>44530</v>
       </c>
       <c r="AQ243">
-        <v>29.643785000000001</v>
+        <v>29.733785000000001</v>
       </c>
     </row>
     <row r="244" spans="42:43" x14ac:dyDescent="0.3">
@@ -14664,7 +14688,7 @@
         <v>44561</v>
       </c>
       <c r="AQ244">
-        <v>29.632444</v>
+        <v>29.722443999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update eikon and historical data
</commit_message>
<xml_diff>
--- a/helper/Eikon.xlsx
+++ b/helper/Eikon.xlsx
@@ -159,70 +159,70 @@
   <volType type="realTimeData">
     <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:41</v>
         <stp/>
-        <stp>{22446A75-6580-49D0-A5C7-EACEE9802E12}_x0000_</stp>
+        <stp>{897E5AF3-EB22-4716-ABC4-2277C539F218}_x0000_</stp>
+        <tr r="M3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:41</v>
+        <stp/>
+        <stp>{AE0C9429-58A1-44FF-8A10-A23081362170}_x0000_</stp>
+        <tr r="I3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:45</v>
+        <stp/>
+        <stp>{F97B50F6-638D-498F-814B-F64D18F20B79}_x0000_</stp>
         <tr r="E3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:44</v>
         <stp/>
-        <stp>{6D9B80F3-934F-48EE-ADEB-8572FFC6E848}_x0000_</stp>
-        <tr r="M3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:05</v>
-        <stp/>
-        <stp>{61D24252-C389-4F55-BA45-CD9258DC1AEE}_x0000_</stp>
+        <stp>{7754FBB4-2365-442C-8F88-BC8397B3BB47}_x0000_</stp>
         <tr r="Y3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:40</v>
         <stp/>
-        <stp>{A3B55305-80C2-4660-8E2E-2D0C3DD639E0}_x0000_</stp>
+        <stp>{79FC90DC-C27E-4D20-8945-B576A7FA8432}_x0000_</stp>
+        <tr r="AK3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:45</v>
+        <stp/>
+        <stp>{249870CF-7B56-489D-B1B3-4D9D9A4208D3}_x0000_</stp>
+        <tr r="A3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:45</v>
+        <stp/>
+        <stp>{9270B0EE-FEB9-4B4D-ADC6-2FB1084CDCA7}_x0000_</stp>
+        <tr r="AC3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:41</v>
+        <stp/>
+        <stp>{CC8A740F-8952-4864-845E-E0E9961890FB}_x0000_</stp>
+        <tr r="Q3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:41</v>
+        <stp/>
+        <stp>{43B9C51B-E4E3-49BA-AE13-29AC6D3D2841}_x0000_</stp>
+        <tr r="AO3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 15:05:41</v>
+        <stp/>
+        <stp>{C9F7E190-13A9-438F-AE92-7B1A8F354EC8}_x0000_</stp>
         <tr r="AG3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:45</v>
         <stp/>
-        <stp>{3B2E30B3-A0E5-4DA2-A9D6-6572FE4A8290}_x0000_</stp>
-        <tr r="Q3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:05</v>
-        <stp/>
-        <stp>{EEC4506D-05E2-48B3-9395-397ACC0456A3}_x0000_</stp>
+        <stp>{0FA8AD9D-92AB-4DD3-AE3E-34A5C8160EBC}_x0000_</stp>
         <tr r="U3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:04</v>
-        <stp/>
-        <stp>{FFC918F4-00C0-4C52-91F2-274825BC9B11}_x0000_</stp>
-        <tr r="I3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:05</v>
-        <stp/>
-        <stp>{81E97F22-8C65-480C-85BC-5745287FFCD7}_x0000_</stp>
-        <tr r="AO3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:04</v>
-        <stp/>
-        <stp>{CDEC0E0D-AEFE-4312-9D4F-3AB226FCD39C}_x0000_</stp>
-        <tr r="AK3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:05</v>
-        <stp/>
-        <stp>{A34ED1E5-C454-4312-9236-F51CDCDDAB13}_x0000_</stp>
-        <tr r="AC3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 09:26:05</v>
-        <stp/>
-        <stp>{0A9CA1AB-86FB-4001-9623-589C8C0415CB}_x0000_</stp>
-        <tr r="A3" s="2"/>
       </tp>
     </main>
   </volType>
@@ -612,47 +612,47 @@
     <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>_xll.RHistory(C2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",B4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:45</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.RHistory(G2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",F4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:45</v>
       </c>
       <c r="I3" t="str">
         <f>_xll.RHistory(K2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",J4)</f>
-        <v>Updated at 09:26:04</v>
+        <v>Updated at 15:05:41</v>
       </c>
       <c r="M3" t="str">
         <f>_xll.RHistory(O2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",N4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:41</v>
       </c>
       <c r="Q3" t="str">
         <f>_xll.RHistory(S2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",R4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:41</v>
       </c>
       <c r="U3" t="str">
         <f>_xll.RHistory(W2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",V4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:45</v>
       </c>
       <c r="Y3" t="str">
         <f>_xll.RHistory(AA2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",Z4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:44</v>
       </c>
       <c r="AC3" t="str">
         <f>_xll.RHistory(AE2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AD4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:45</v>
       </c>
       <c r="AG3" t="str">
         <f>_xll.RHistory(AI2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AH4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:41</v>
       </c>
       <c r="AK3" t="str">
         <f>_xll.RHistory(AM2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AL4)</f>
-        <v>Updated at 09:26:04</v>
+        <v>Updated at 15:05:40</v>
       </c>
       <c r="AO3" t="str">
         <f>_xll.RHistory(AQ2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AP4)</f>
-        <v>Updated at 09:26:05</v>
+        <v>Updated at 15:05:41</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.3">
@@ -5134,7 +5134,7 @@
         <v>43982</v>
       </c>
       <c r="AM69">
-        <v>19053.14</v>
+        <v>18947.77</v>
       </c>
       <c r="AP69" s="2">
         <v>39233</v>
@@ -5202,7 +5202,7 @@
         <v>44012</v>
       </c>
       <c r="AM70">
-        <v>16987.62</v>
+        <v>17028.66</v>
       </c>
       <c r="AP70" s="2">
         <v>39263</v>
@@ -5270,7 +5270,7 @@
         <v>44043</v>
       </c>
       <c r="AM71">
-        <v>18367.54</v>
+        <v>18322.32</v>
       </c>
       <c r="AP71" s="2">
         <v>39294</v>
@@ -5338,7 +5338,7 @@
         <v>44074</v>
       </c>
       <c r="AM72">
-        <v>17942.7</v>
+        <v>18609.169999999998</v>
       </c>
       <c r="AP72" s="2">
         <v>39325</v>
@@ -5402,6 +5402,12 @@
       <c r="AI73">
         <v>1059246</v>
       </c>
+      <c r="AL73" s="2">
+        <v>44104</v>
+      </c>
+      <c r="AM73">
+        <v>10074.34</v>
+      </c>
       <c r="AP73" s="2">
         <v>39355</v>
       </c>
@@ -14536,6 +14542,12 @@
       <c r="AE227">
         <v>54.2</v>
       </c>
+      <c r="AH227" s="2">
+        <v>44043</v>
+      </c>
+      <c r="AI227">
+        <v>0</v>
+      </c>
       <c r="AP227" s="2">
         <v>44043</v>
       </c>
@@ -14548,13 +14560,25 @@
         <v>44074</v>
       </c>
       <c r="O228">
-        <v>1518</v>
+        <v>1488</v>
       </c>
       <c r="R228" s="2">
         <v>44074</v>
       </c>
       <c r="S228">
-        <v>597</v>
+        <v>666</v>
+      </c>
+      <c r="V228" s="2">
+        <v>44074</v>
+      </c>
+      <c r="W228">
+        <v>56</v>
+      </c>
+      <c r="AD228" s="2">
+        <v>44074</v>
+      </c>
+      <c r="AE228">
+        <v>55.2</v>
       </c>
       <c r="AP228" s="2">
         <v>44074</v>
@@ -14564,6 +14588,12 @@
       </c>
     </row>
     <row r="229" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="N229" s="2">
+        <v>44104</v>
+      </c>
+      <c r="O229">
+        <v>1471</v>
+      </c>
       <c r="AP229" s="2">
         <v>44104</v>
       </c>

</xml_diff>

<commit_message>
rename emerging asia cpb, add eikon data
</commit_message>
<xml_diff>
--- a/helper/Eikon.xlsx
+++ b/helper/Eikon.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\C\Users\Nour.Barnat\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maystre\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B928CEF9-13F4-423C-8400-7A830CD8B9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="312" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18240" windowHeight="28590" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eikon" sheetId="2" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="TRNR_45b48680f2074c1e847365beb09c7c6c_25_1" hidden="1">Eikon!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -88,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,70 +161,70 @@
   <volType type="realTimeData">
     <main first="pldatasource.rhistoryrtdserver">
       <tp t="s">
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:57</v>
         <stp/>
-        <stp>{1B1C3A74-D50C-462B-9D12-47D8E44BAA43}_x0000_</stp>
+        <stp>{1820C474-B27F-4DD8-A817-3024F662DD60}_x0000_</stp>
+        <tr r="A3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:16:50</v>
+        <stp/>
+        <stp>{69BA9DCE-BE0F-4A47-BFEB-42FC75EB1369}_x0000_</stp>
+        <tr r="AG3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:16:51</v>
+        <stp/>
+        <stp>{C9DD2D8C-F9CB-4069-9E94-6CBD2C41B963}_x0000_</stp>
+        <tr r="AO3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:16:52</v>
+        <stp/>
+        <stp>{60F6AA2E-298A-4F87-B5CA-9C5F229FB9D8}_x0000_</stp>
         <tr r="AK3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:51</v>
         <stp/>
-        <stp>{B9BA6245-81B0-457C-BFAB-CFAF0850D407}_x0000_</stp>
+        <stp>{8CB438A2-F1AD-476F-B968-1D9C081A3F1A}_x0000_</stp>
+        <tr r="M3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:16:51</v>
+        <stp/>
+        <stp>{F4621E88-E37E-4E91-8512-BF4FA171BEDD}_x0000_</stp>
+        <tr r="AC3" s="2"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 12:16:50</v>
+        <stp/>
+        <stp>{A8D534AA-2CAE-4478-A3A1-CEC53648AB71}_x0000_</stp>
         <tr r="Y3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:57</v>
         <stp/>
-        <stp>{6CDF3B86-F3EC-4AC5-8509-DBD5EAABF1D8}_x0000_</stp>
-        <tr r="AC3" s="2"/>
+        <stp>{A89C752C-32A2-42DF-857C-E524A4AA78DA}_x0000_</stp>
+        <tr r="E3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:51</v>
         <stp/>
-        <stp>{B9E17866-665F-4982-8210-D6A7D75857F3}_x0000_</stp>
-        <tr r="AO3" s="2"/>
+        <stp>{4BDF656C-7285-41C8-B641-4EB2ECBDC2DF}_x0000_</stp>
+        <tr r="I3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:57</v>
         <stp/>
-        <stp>{47102A40-06B5-4A76-892B-E80E49EEC694}_x0000_</stp>
-        <tr r="M3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:03:13</v>
-        <stp/>
-        <stp>{B456A10A-A14A-4911-9AC5-6FEDBBA03149}_x0000_</stp>
-        <tr r="Q3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:03:12</v>
-        <stp/>
-        <stp>{CE273B56-5A80-478A-B98F-BA5F4F562222}_x0000_</stp>
+        <stp>{B8667DD7-E6E7-4E3D-B30F-E338FA110BE3}_x0000_</stp>
         <tr r="U3" s="2"/>
       </tp>
       <tp t="s">
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:49</v>
         <stp/>
-        <stp>{F4BBBF19-CCB9-4CE0-885D-83423C8C061B}_x0000_</stp>
-        <tr r="I3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:03:13</v>
-        <stp/>
-        <stp>{D26E879D-1F40-4368-A41B-1690833504E0}_x0000_</stp>
-        <tr r="A3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>Updated at 12:03:14</v>
-        <stp/>
-        <stp>{FB5D6E62-9BE9-4828-8442-C95ACA894DE6}_x0000_</stp>
-        <tr r="E3" s="2"/>
-      </tp>
-      <tp t="s">
-        <v>The time series server does not have enough resources to complete the request for: aTHTOURIAR</v>
-        <stp/>
-        <stp>{238EAF94-1F9C-4425-8ECC-2CF262B605C9}_x0000_</stp>
-        <tr r="AG3" s="2"/>
+        <stp>{BAF8C946-5F7E-40B7-A0C0-6454CD3A1C4E}_x0000_</stp>
+        <tr r="Q3" s="2"/>
       </tp>
     </main>
   </volType>
@@ -525,33 +527,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AQ244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" customWidth="1"/>
-    <col min="22" max="22" width="11.109375" customWidth="1"/>
-    <col min="25" max="27" width="12.6640625" customWidth="1"/>
-    <col min="29" max="31" width="12.6640625" customWidth="1"/>
-    <col min="33" max="35" width="12.6640625" customWidth="1"/>
-    <col min="37" max="39" width="12.6640625" customWidth="1"/>
-    <col min="41" max="43" width="12.6640625" customWidth="1"/>
+    <col min="1" max="3" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" customWidth="1"/>
+    <col min="22" max="22" width="11.140625" customWidth="1"/>
+    <col min="25" max="27" width="12.7109375" customWidth="1"/>
+    <col min="29" max="31" width="12.7109375" customWidth="1"/>
+    <col min="33" max="35" width="12.7109375" customWidth="1"/>
+    <col min="37" max="39" width="12.7109375" customWidth="1"/>
+    <col min="41" max="43" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="M1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
@@ -573,7 +575,7 @@
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
@@ -609,53 +611,53 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>_xll.RHistory(C2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",B4)</f>
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:57</v>
       </c>
       <c r="E3" t="str">
         <f>_xll.RHistory(G2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",F4)</f>
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:57</v>
       </c>
       <c r="I3" t="str">
         <f>_xll.RHistory(K2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:NO SORT:ASC NULL:NA CH:Fd",J4)</f>
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:51</v>
       </c>
       <c r="M3" t="str">
         <f>_xll.RHistory(O2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",N4)</f>
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:51</v>
       </c>
       <c r="Q3" t="str">
         <f>_xll.RHistory(S2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",R4)</f>
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:49</v>
       </c>
       <c r="U3" t="str">
         <f>_xll.RHistory(W2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",V4)</f>
-        <v>Updated at 12:03:12</v>
+        <v>Updated at 12:16:57</v>
       </c>
       <c r="Y3" t="str">
         <f>_xll.RHistory(AA2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",Z4)</f>
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:50</v>
       </c>
       <c r="AC3" t="str">
         <f>_xll.RHistory(AE2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AD4)</f>
-        <v>Updated at 12:03:14</v>
+        <v>Updated at 12:16:51</v>
       </c>
       <c r="AG3" t="str">
         <f>_xll.RHistory(AI2,"ECONOMIC.Timestamp;ECONOMIC.Value","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC NULL:NA CH:Fd",AH4)</f>
-        <v>The time series server does not have enough resources to complete the request for: aTHTOURIAR</v>
+        <v>Updated at 12:16:50</v>
       </c>
       <c r="AK3" t="str">
         <f>_xll.RHistory(AM2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AL4)</f>
-        <v>Updated at 12:03:13</v>
+        <v>Updated at 12:16:52</v>
       </c>
       <c r="AO3" t="str">
         <f>_xll.RHistory(AQ2,".Timestamp;.Close","START:01-Jan-2002 INTERVAL:1MO",,"TSREPEAT:YES SORT:ASC CH:Fd",AP4)</f>
-        <v>Updated at 12:03:14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+        <v>Updated at 12:16:51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -723,7 +725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>37287</v>
       </c>
@@ -791,7 +793,7 @@
         <v>27.31</v>
       </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>37315</v>
       </c>
@@ -859,7 +861,7 @@
         <v>27.82</v>
       </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>37346</v>
       </c>
@@ -927,7 +929,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>37376</v>
       </c>
@@ -995,7 +997,7 @@
         <v>26.97</v>
       </c>
     </row>
-    <row r="9" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>37407</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>26.88</v>
       </c>
     </row>
-    <row r="10" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>37437</v>
       </c>
@@ -1131,7 +1133,7 @@
         <v>25.98</v>
       </c>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>37468</v>
       </c>
@@ -1199,7 +1201,7 @@
         <v>25.47</v>
       </c>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>37499</v>
       </c>
@@ -1267,7 +1269,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>37529</v>
       </c>
@@ -1335,7 +1337,7 @@
         <v>25.71</v>
       </c>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>37560</v>
       </c>
@@ -1403,7 +1405,7 @@
         <v>24.51</v>
       </c>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>37590</v>
       </c>
@@ -1471,7 +1473,7 @@
         <v>25.35</v>
       </c>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:43" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>37621</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>25.07</v>
       </c>
     </row>
-    <row r="17" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>37652</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>25.65</v>
       </c>
     </row>
-    <row r="18" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>37680</v>
       </c>
@@ -1675,7 +1677,7 @@
         <v>25.5</v>
       </c>
     </row>
-    <row r="19" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>37711</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>26.32</v>
       </c>
     </row>
-    <row r="20" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>37741</v>
       </c>
@@ -1811,7 +1813,7 @@
         <v>27.07</v>
       </c>
     </row>
-    <row r="21" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>37772</v>
       </c>
@@ -1879,7 +1881,7 @@
         <v>27.14</v>
       </c>
     </row>
-    <row r="22" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>37802</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>25.34</v>
       </c>
     </row>
-    <row r="23" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>37833</v>
       </c>
@@ -2015,7 +2017,7 @@
         <v>25.75</v>
       </c>
     </row>
-    <row r="24" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>37864</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>27.04</v>
       </c>
     </row>
-    <row r="25" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>37894</v>
       </c>
@@ -2151,7 +2153,7 @@
         <v>27.66</v>
       </c>
     </row>
-    <row r="26" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>37925</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>26.86</v>
       </c>
     </row>
-    <row r="27" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>37955</v>
       </c>
@@ -2287,7 +2289,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>37986</v>
       </c>
@@ -2355,7 +2357,7 @@
         <v>26.32</v>
       </c>
     </row>
-    <row r="29" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>38017</v>
       </c>
@@ -2423,7 +2425,7 @@
         <v>26.46</v>
       </c>
     </row>
-    <row r="30" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>38046</v>
       </c>
@@ -2491,7 +2493,7 @@
         <v>26.95</v>
       </c>
     </row>
-    <row r="31" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>38077</v>
       </c>
@@ -2559,7 +2561,7 @@
         <v>27.39</v>
       </c>
     </row>
-    <row r="32" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>38107</v>
       </c>
@@ -2627,7 +2629,7 @@
         <v>28.01</v>
       </c>
     </row>
-    <row r="33" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>38138</v>
       </c>
@@ -2695,7 +2697,7 @@
         <v>28.01</v>
       </c>
     </row>
-    <row r="34" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>38168</v>
       </c>
@@ -2763,7 +2765,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="35" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>38199</v>
       </c>
@@ -2831,7 +2833,7 @@
         <v>28.98</v>
       </c>
     </row>
-    <row r="36" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>38230</v>
       </c>
@@ -2899,7 +2901,7 @@
         <v>28.92</v>
       </c>
     </row>
-    <row r="37" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>38260</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="38" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>38291</v>
       </c>
@@ -3035,7 +3037,7 @@
         <v>28.77</v>
       </c>
     </row>
-    <row r="39" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>38321</v>
       </c>
@@ -3103,7 +3105,7 @@
         <v>28.59</v>
       </c>
     </row>
-    <row r="40" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>38352</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>29.72</v>
       </c>
     </row>
-    <row r="41" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>38383</v>
       </c>
@@ -3239,7 +3241,7 @@
         <v>30.12</v>
       </c>
     </row>
-    <row r="42" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>38411</v>
       </c>
@@ -3307,7 +3309,7 @@
         <v>29.93</v>
       </c>
     </row>
-    <row r="43" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>38442</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>30.45</v>
       </c>
     </row>
-    <row r="44" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
         <v>38472</v>
       </c>
@@ -3443,7 +3445,7 @@
         <v>30.48</v>
       </c>
     </row>
-    <row r="45" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
         <v>38503</v>
       </c>
@@ -3511,7 +3513,7 @@
         <v>29.95</v>
       </c>
     </row>
-    <row r="46" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
         <v>38533</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>30.15</v>
       </c>
     </row>
-    <row r="47" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
         <v>38564</v>
       </c>
@@ -3647,7 +3649,7 @@
         <v>30.35</v>
       </c>
     </row>
-    <row r="48" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
         <v>38595</v>
       </c>
@@ -3715,7 +3717,7 @@
         <v>30.46</v>
       </c>
     </row>
-    <row r="49" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
         <v>38625</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>30.65</v>
       </c>
     </row>
-    <row r="50" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
         <v>38656</v>
       </c>
@@ -3851,7 +3853,7 @@
         <v>30.76</v>
       </c>
     </row>
-    <row r="51" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
         <v>38686</v>
       </c>
@@ -3919,7 +3921,7 @@
         <v>30.64</v>
       </c>
     </row>
-    <row r="52" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
         <v>38717</v>
       </c>
@@ -3987,7 +3989,7 @@
         <v>30.78</v>
       </c>
     </row>
-    <row r="53" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
         <v>38748</v>
       </c>
@@ -4055,7 +4057,7 @@
         <v>31.03</v>
       </c>
     </row>
-    <row r="54" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
         <v>38776</v>
       </c>
@@ -4123,7 +4125,7 @@
         <v>30.99</v>
       </c>
     </row>
-    <row r="55" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
         <v>38807</v>
       </c>
@@ -4191,7 +4193,7 @@
         <v>31.38</v>
       </c>
     </row>
-    <row r="56" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
         <v>38837</v>
       </c>
@@ -4259,7 +4261,7 @@
         <v>31.03</v>
       </c>
     </row>
-    <row r="57" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
         <v>38868</v>
       </c>
@@ -4327,7 +4329,7 @@
         <v>30.98</v>
       </c>
     </row>
-    <row r="58" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
         <v>38898</v>
       </c>
@@ -4395,7 +4397,7 @@
         <v>30.91</v>
       </c>
     </row>
-    <row r="59" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
         <v>38929</v>
       </c>
@@ -4463,7 +4465,7 @@
         <v>30.61</v>
       </c>
     </row>
-    <row r="60" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
         <v>38960</v>
       </c>
@@ -4531,7 +4533,7 @@
         <v>30.64</v>
       </c>
     </row>
-    <row r="61" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
         <v>38990</v>
       </c>
@@ -4599,7 +4601,7 @@
         <v>30.47</v>
       </c>
     </row>
-    <row r="62" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
         <v>39021</v>
       </c>
@@ -4667,7 +4669,7 @@
         <v>30.49</v>
       </c>
     </row>
-    <row r="63" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
         <v>39051</v>
       </c>
@@ -4735,7 +4737,7 @@
         <v>30.17</v>
       </c>
     </row>
-    <row r="64" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
         <v>39082</v>
       </c>
@@ -4803,7 +4805,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="65" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
         <v>39113</v>
       </c>
@@ -4871,7 +4873,7 @@
         <v>30.73</v>
       </c>
     </row>
-    <row r="66" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
         <v>39141</v>
       </c>
@@ -4939,7 +4941,7 @@
         <v>30.83</v>
       </c>
     </row>
-    <row r="67" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
         <v>39172</v>
       </c>
@@ -5007,7 +5009,7 @@
         <v>30.48</v>
       </c>
     </row>
-    <row r="68" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
         <v>39202</v>
       </c>
@@ -5075,7 +5077,7 @@
         <v>30.24</v>
       </c>
     </row>
-    <row r="69" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
         <v>39233</v>
       </c>
@@ -5143,7 +5145,7 @@
         <v>29.86</v>
       </c>
     </row>
-    <row r="70" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
         <v>39263</v>
       </c>
@@ -5211,7 +5213,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="71" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
         <v>39294</v>
       </c>
@@ -5279,7 +5281,7 @@
         <v>29.48</v>
       </c>
     </row>
-    <row r="72" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
         <v>39325</v>
       </c>
@@ -5347,7 +5349,7 @@
         <v>29.54</v>
       </c>
     </row>
-    <row r="73" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
         <v>39355</v>
       </c>
@@ -5406,7 +5408,7 @@
         <v>44104</v>
       </c>
       <c r="AM73">
-        <v>18713.310000000001</v>
+        <v>18748.849999999999</v>
       </c>
       <c r="AP73" s="2">
         <v>39355</v>
@@ -5415,7 +5417,7 @@
         <v>29.59</v>
       </c>
     </row>
-    <row r="74" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
         <v>39386</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>44135</v>
       </c>
       <c r="AM74">
-        <v>16675.03</v>
+        <v>17116.93</v>
       </c>
       <c r="AP74" s="2">
         <v>39386</v>
@@ -5483,7 +5485,7 @@
         <v>29.82</v>
       </c>
     </row>
-    <row r="75" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
         <v>39416</v>
       </c>
@@ -5545,7 +5547,7 @@
         <v>29.65</v>
       </c>
     </row>
-    <row r="76" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
         <v>39447</v>
       </c>
@@ -5607,7 +5609,7 @@
         <v>29.52</v>
       </c>
     </row>
-    <row r="77" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
         <v>39478</v>
       </c>
@@ -5669,7 +5671,7 @@
         <v>29.78</v>
       </c>
     </row>
-    <row r="78" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
         <v>39507</v>
       </c>
@@ -5731,7 +5733,7 @@
         <v>29.76</v>
       </c>
     </row>
-    <row r="79" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
         <v>39538</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>30.41</v>
       </c>
     </row>
-    <row r="80" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
         <v>39568</v>
       </c>
@@ -5855,7 +5857,7 @@
         <v>30.59</v>
       </c>
     </row>
-    <row r="81" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
         <v>39599</v>
       </c>
@@ -5917,7 +5919,7 @@
         <v>30.44</v>
       </c>
     </row>
-    <row r="82" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
         <v>39629</v>
       </c>
@@ -5979,7 +5981,7 @@
         <v>31.11</v>
       </c>
     </row>
-    <row r="83" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B83" s="2">
         <v>39660</v>
       </c>
@@ -6041,7 +6043,7 @@
         <v>31.08</v>
       </c>
     </row>
-    <row r="84" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B84" s="2">
         <v>39691</v>
       </c>
@@ -6103,7 +6105,7 @@
         <v>31.16</v>
       </c>
     </row>
-    <row r="85" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
         <v>39721</v>
       </c>
@@ -6165,7 +6167,7 @@
         <v>31.36</v>
       </c>
     </row>
-    <row r="86" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
         <v>39752</v>
       </c>
@@ -6227,7 +6229,7 @@
         <v>31.07</v>
       </c>
     </row>
-    <row r="87" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
         <v>39782</v>
       </c>
@@ -6289,7 +6291,7 @@
         <v>31.42</v>
       </c>
     </row>
-    <row r="88" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B88" s="2">
         <v>39813</v>
       </c>
@@ -6351,7 +6353,7 @@
         <v>31.49</v>
       </c>
     </row>
-    <row r="89" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B89" s="2">
         <v>39844</v>
       </c>
@@ -6413,7 +6415,7 @@
         <v>31.86</v>
       </c>
     </row>
-    <row r="90" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
         <v>39872</v>
       </c>
@@ -6475,7 +6477,7 @@
         <v>31.67</v>
       </c>
     </row>
-    <row r="91" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
         <v>39903</v>
       </c>
@@ -6537,7 +6539,7 @@
         <v>31.36</v>
       </c>
     </row>
-    <row r="92" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
         <v>39933</v>
       </c>
@@ -6599,7 +6601,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="93" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
         <v>39964</v>
       </c>
@@ -6661,7 +6663,7 @@
         <v>30.69</v>
       </c>
     </row>
-    <row r="94" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
         <v>39994</v>
       </c>
@@ -6723,7 +6725,7 @@
         <v>30.05</v>
       </c>
     </row>
-    <row r="95" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
         <v>40025</v>
       </c>
@@ -6785,7 +6787,7 @@
         <v>29.08</v>
       </c>
     </row>
-    <row r="96" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
         <v>40056</v>
       </c>
@@ -6847,7 +6849,7 @@
         <v>28.92</v>
       </c>
     </row>
-    <row r="97" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
         <v>40086</v>
       </c>
@@ -6909,7 +6911,7 @@
         <v>28.81</v>
       </c>
     </row>
-    <row r="98" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
         <v>40117</v>
       </c>
@@ -6971,7 +6973,7 @@
         <v>28.96</v>
       </c>
     </row>
-    <row r="99" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
         <v>40147</v>
       </c>
@@ -7033,7 +7035,7 @@
         <v>28.97</v>
       </c>
     </row>
-    <row r="100" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
         <v>40178</v>
       </c>
@@ -7095,7 +7097,7 @@
         <v>29.06</v>
       </c>
     </row>
-    <row r="101" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
         <v>40209</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>29.29</v>
       </c>
     </row>
-    <row r="102" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
         <v>40237</v>
       </c>
@@ -7219,7 +7221,7 @@
         <v>29.38</v>
       </c>
     </row>
-    <row r="103" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
         <v>40268</v>
       </c>
@@ -7281,7 +7283,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="104" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B104" s="2">
         <v>40298</v>
       </c>
@@ -7343,7 +7345,7 @@
         <v>29.44</v>
       </c>
     </row>
-    <row r="105" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B105" s="2">
         <v>40329</v>
       </c>
@@ -7405,7 +7407,7 @@
         <v>29.48</v>
       </c>
     </row>
-    <row r="106" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B106" s="2">
         <v>40359</v>
       </c>
@@ -7467,7 +7469,7 @@
         <v>29.45</v>
       </c>
     </row>
-    <row r="107" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B107" s="2">
         <v>40390</v>
       </c>
@@ -7529,7 +7531,7 @@
         <v>29.44</v>
       </c>
     </row>
-    <row r="108" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B108" s="2">
         <v>40421</v>
       </c>
@@ -7591,7 +7593,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="109" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B109" s="2">
         <v>40451</v>
       </c>
@@ -7653,7 +7655,7 @@
         <v>29.67</v>
       </c>
     </row>
-    <row r="110" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B110" s="2">
         <v>40482</v>
       </c>
@@ -7715,7 +7717,7 @@
         <v>29.81</v>
       </c>
     </row>
-    <row r="111" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B111" s="2">
         <v>40512</v>
       </c>
@@ -7777,7 +7779,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="112" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B112" s="2">
         <v>40543</v>
       </c>
@@ -7839,7 +7841,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="113" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B113" s="2">
         <v>40574</v>
       </c>
@@ -7901,7 +7903,7 @@
         <v>30.35</v>
       </c>
     </row>
-    <row r="114" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B114" s="2">
         <v>40602</v>
       </c>
@@ -7963,7 +7965,7 @@
         <v>30.31</v>
       </c>
     </row>
-    <row r="115" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B115" s="2">
         <v>40633</v>
       </c>
@@ -8025,7 +8027,7 @@
         <v>30.3</v>
       </c>
     </row>
-    <row r="116" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B116" s="2">
         <v>40663</v>
       </c>
@@ -8087,7 +8089,7 @@
         <v>29.79</v>
       </c>
     </row>
-    <row r="117" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B117" s="2">
         <v>40694</v>
       </c>
@@ -8149,7 +8151,7 @@
         <v>29.93</v>
       </c>
     </row>
-    <row r="118" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B118" s="2">
         <v>40724</v>
       </c>
@@ -8211,7 +8213,7 @@
         <v>29.96</v>
       </c>
     </row>
-    <row r="119" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B119" s="2">
         <v>40755</v>
       </c>
@@ -8273,7 +8275,7 @@
         <v>30.55</v>
       </c>
     </row>
-    <row r="120" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B120" s="2">
         <v>40786</v>
       </c>
@@ -8335,7 +8337,7 @@
         <v>30.08</v>
       </c>
     </row>
-    <row r="121" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B121" s="2">
         <v>40816</v>
       </c>
@@ -8397,7 +8399,7 @@
         <v>28.87</v>
       </c>
     </row>
-    <row r="122" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B122" s="2">
         <v>40847</v>
       </c>
@@ -8459,7 +8461,7 @@
         <v>28.92</v>
       </c>
     </row>
-    <row r="123" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B123" s="2">
         <v>40877</v>
       </c>
@@ -8521,7 +8523,7 @@
         <v>29.01</v>
       </c>
     </row>
-    <row r="124" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B124" s="2">
         <v>40908</v>
       </c>
@@ -8583,7 +8585,7 @@
         <v>29.65</v>
       </c>
     </row>
-    <row r="125" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B125" s="2">
         <v>40939</v>
       </c>
@@ -8645,7 +8647,7 @@
         <v>29.93</v>
       </c>
     </row>
-    <row r="126" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B126" s="2">
         <v>40968</v>
       </c>
@@ -8707,7 +8709,7 @@
         <v>30.02</v>
       </c>
     </row>
-    <row r="127" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B127" s="2">
         <v>40999</v>
       </c>
@@ -8769,7 +8771,7 @@
         <v>30.09</v>
       </c>
     </row>
-    <row r="128" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B128" s="2">
         <v>41029</v>
       </c>
@@ -8831,7 +8833,7 @@
         <v>29.77</v>
       </c>
     </row>
-    <row r="129" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B129" s="2">
         <v>41060</v>
       </c>
@@ -8893,7 +8895,7 @@
         <v>30.63</v>
       </c>
     </row>
-    <row r="130" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B130" s="2">
         <v>41090</v>
       </c>
@@ -8955,7 +8957,7 @@
         <v>30.61</v>
       </c>
     </row>
-    <row r="131" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B131" s="2">
         <v>41121</v>
       </c>
@@ -9017,7 +9019,7 @@
         <v>30.82</v>
       </c>
     </row>
-    <row r="132" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B132" s="2">
         <v>41152</v>
       </c>
@@ -9079,7 +9081,7 @@
         <v>31.11</v>
       </c>
     </row>
-    <row r="133" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B133" s="2">
         <v>41182</v>
       </c>
@@ -9141,7 +9143,7 @@
         <v>31.32</v>
       </c>
     </row>
-    <row r="134" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
         <v>41213</v>
       </c>
@@ -9203,7 +9205,7 @@
         <v>31.56</v>
       </c>
     </row>
-    <row r="135" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
         <v>41243</v>
       </c>
@@ -9265,7 +9267,7 @@
         <v>31.16</v>
       </c>
     </row>
-    <row r="136" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B136" s="2">
         <v>41274</v>
       </c>
@@ -9327,7 +9329,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="137" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B137" s="2">
         <v>41305</v>
       </c>
@@ -9389,7 +9391,7 @@
         <v>31.14</v>
       </c>
     </row>
-    <row r="138" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B138" s="2">
         <v>41333</v>
       </c>
@@ -9451,7 +9453,7 @@
         <v>31.32</v>
       </c>
     </row>
-    <row r="139" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B139" s="2">
         <v>41364</v>
       </c>
@@ -9513,7 +9515,7 @@
         <v>31.11</v>
       </c>
     </row>
-    <row r="140" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B140" s="2">
         <v>41394</v>
       </c>
@@ -9575,7 +9577,7 @@
         <v>30.65</v>
       </c>
     </row>
-    <row r="141" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B141" s="2">
         <v>41425</v>
       </c>
@@ -9637,7 +9639,7 @@
         <v>30.57</v>
       </c>
     </row>
-    <row r="142" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B142" s="2">
         <v>41455</v>
       </c>
@@ -9699,7 +9701,7 @@
         <v>30.15</v>
       </c>
     </row>
-    <row r="143" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B143" s="2">
         <v>41486</v>
       </c>
@@ -9761,7 +9763,7 @@
         <v>29.91</v>
       </c>
     </row>
-    <row r="144" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B144" s="2">
         <v>41517</v>
       </c>
@@ -9823,7 +9825,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="145" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B145" s="2">
         <v>41547</v>
       </c>
@@ -9885,7 +9887,7 @@
         <v>29.96</v>
       </c>
     </row>
-    <row r="146" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B146" s="2">
         <v>41578</v>
       </c>
@@ -9947,7 +9949,7 @@
         <v>30.42</v>
       </c>
     </row>
-    <row r="147" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B147" s="2">
         <v>41608</v>
       </c>
@@ -10009,7 +10011,7 @@
         <v>30.39</v>
       </c>
     </row>
-    <row r="148" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B148" s="2">
         <v>41639</v>
       </c>
@@ -10071,7 +10073,7 @@
         <v>30.28</v>
       </c>
     </row>
-    <row r="149" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B149" s="2">
         <v>41670</v>
       </c>
@@ -10133,7 +10135,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="150" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B150" s="2">
         <v>41698</v>
       </c>
@@ -10195,7 +10197,7 @@
         <v>30.47</v>
       </c>
     </row>
-    <row r="151" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B151" s="2">
         <v>41729</v>
       </c>
@@ -10257,7 +10259,7 @@
         <v>29.65</v>
       </c>
     </row>
-    <row r="152" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B152" s="2">
         <v>41759</v>
       </c>
@@ -10319,7 +10321,7 @@
         <v>29.62</v>
       </c>
     </row>
-    <row r="153" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B153" s="2">
         <v>41790</v>
       </c>
@@ -10381,7 +10383,7 @@
         <v>29.12</v>
       </c>
     </row>
-    <row r="154" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B154" s="2">
         <v>41820</v>
       </c>
@@ -10443,7 +10445,7 @@
         <v>29.31</v>
       </c>
     </row>
-    <row r="155" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B155" s="2">
         <v>41851</v>
       </c>
@@ -10505,7 +10507,7 @@
         <v>29.83</v>
       </c>
     </row>
-    <row r="156" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B156" s="2">
         <v>41882</v>
       </c>
@@ -10567,7 +10569,7 @@
         <v>29.97</v>
       </c>
     </row>
-    <row r="157" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B157" s="2">
         <v>41912</v>
       </c>
@@ -10629,7 +10631,7 @@
         <v>29.48</v>
       </c>
     </row>
-    <row r="158" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B158" s="2">
         <v>41943</v>
       </c>
@@ -10691,7 +10693,7 @@
         <v>29.32</v>
       </c>
     </row>
-    <row r="159" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B159" s="2">
         <v>41973</v>
       </c>
@@ -10753,7 +10755,7 @@
         <v>29.62</v>
       </c>
     </row>
-    <row r="160" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B160" s="2">
         <v>42004</v>
       </c>
@@ -10815,7 +10817,7 @@
         <v>29.64</v>
       </c>
     </row>
-    <row r="161" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B161" s="2">
         <v>42035</v>
       </c>
@@ -10877,7 +10879,7 @@
         <v>30.064392999999999</v>
       </c>
     </row>
-    <row r="162" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B162" s="2">
         <v>42063</v>
       </c>
@@ -10939,7 +10941,7 @@
         <v>29.958182000000001</v>
       </c>
     </row>
-    <row r="163" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B163" s="2">
         <v>42094</v>
       </c>
@@ -11001,7 +11003,7 @@
         <v>30.790761</v>
       </c>
     </row>
-    <row r="164" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B164" s="2">
         <v>42124</v>
       </c>
@@ -11057,7 +11059,7 @@
         <v>30.939561999999999</v>
       </c>
     </row>
-    <row r="165" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B165" s="2">
         <v>42155</v>
       </c>
@@ -11113,7 +11115,7 @@
         <v>31.184722000000001</v>
       </c>
     </row>
-    <row r="166" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B166" s="2">
         <v>42185</v>
       </c>
@@ -11169,7 +11171,7 @@
         <v>31.633790999999999</v>
       </c>
     </row>
-    <row r="167" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B167" s="2">
         <v>42216</v>
       </c>
@@ -11225,7 +11227,7 @@
         <v>31.838521</v>
       </c>
     </row>
-    <row r="168" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B168" s="2">
         <v>42247</v>
       </c>
@@ -11281,7 +11283,7 @@
         <v>31.624684999999999</v>
       </c>
     </row>
-    <row r="169" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B169" s="2">
         <v>42277</v>
       </c>
@@ -11337,7 +11339,7 @@
         <v>31.755617999999998</v>
       </c>
     </row>
-    <row r="170" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B170" s="2">
         <v>42308</v>
       </c>
@@ -11393,7 +11395,7 @@
         <v>31.529555999999999</v>
       </c>
     </row>
-    <row r="171" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B171" s="2">
         <v>42338</v>
       </c>
@@ -11449,7 +11451,7 @@
         <v>31.653449999999999</v>
       </c>
     </row>
-    <row r="172" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B172" s="2">
         <v>42369</v>
       </c>
@@ -11505,7 +11507,7 @@
         <v>31.637356</v>
       </c>
     </row>
-    <row r="173" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B173" s="2">
         <v>42400</v>
       </c>
@@ -11561,7 +11563,7 @@
         <v>31.489542</v>
       </c>
     </row>
-    <row r="174" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B174" s="2">
         <v>42429</v>
       </c>
@@ -11617,7 +11619,7 @@
         <v>31.065529999999999</v>
       </c>
     </row>
-    <row r="175" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B175" s="2">
         <v>42460</v>
       </c>
@@ -11673,7 +11675,7 @@
         <v>31.159545000000001</v>
       </c>
     </row>
-    <row r="176" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B176" s="2">
         <v>42490</v>
       </c>
@@ -11729,7 +11731,7 @@
         <v>31.266058000000001</v>
       </c>
     </row>
-    <row r="177" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B177" s="2">
         <v>42521</v>
       </c>
@@ -11785,7 +11787,7 @@
         <v>31.291350999999999</v>
       </c>
     </row>
-    <row r="178" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B178" s="2">
         <v>42551</v>
       </c>
@@ -11841,7 +11843,7 @@
         <v>31.725463000000001</v>
       </c>
     </row>
-    <row r="179" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B179" s="2">
         <v>42582</v>
       </c>
@@ -11897,7 +11899,7 @@
         <v>31.809995000000001</v>
       </c>
     </row>
-    <row r="180" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B180" s="2">
         <v>42613</v>
       </c>
@@ -11953,7 +11955,7 @@
         <v>31.683743</v>
       </c>
     </row>
-    <row r="181" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B181" s="2">
         <v>42643</v>
       </c>
@@ -12009,7 +12011,7 @@
         <v>31.735520000000001</v>
       </c>
     </row>
-    <row r="182" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B182" s="2">
         <v>42674</v>
       </c>
@@ -12065,7 +12067,7 @@
         <v>31.999327000000001</v>
       </c>
     </row>
-    <row r="183" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B183" s="2">
         <v>42704</v>
       </c>
@@ -12121,7 +12123,7 @@
         <v>32.391314999999999</v>
       </c>
     </row>
-    <row r="184" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B184" s="2">
         <v>42735</v>
       </c>
@@ -12177,7 +12179,7 @@
         <v>32.249707999999998</v>
       </c>
     </row>
-    <row r="185" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B185" s="2">
         <v>42766</v>
       </c>
@@ -12233,7 +12235,7 @@
         <v>31.31</v>
       </c>
     </row>
-    <row r="186" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B186" s="2">
         <v>42794</v>
       </c>
@@ -12289,7 +12291,7 @@
         <v>31.192</v>
       </c>
     </row>
-    <row r="187" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B187" s="2">
         <v>42825</v>
       </c>
@@ -12345,7 +12347,7 @@
         <v>30.815000000000001</v>
       </c>
     </row>
-    <row r="188" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B188" s="2">
         <v>42855</v>
       </c>
@@ -12401,7 +12403,7 @@
         <v>30.896000000000001</v>
       </c>
     </row>
-    <row r="189" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B189" s="2">
         <v>42886</v>
       </c>
@@ -12457,7 +12459,7 @@
         <v>31.399000000000001</v>
       </c>
     </row>
-    <row r="190" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B190" s="2">
         <v>42916</v>
       </c>
@@ -12513,7 +12515,7 @@
         <v>31.83</v>
       </c>
     </row>
-    <row r="191" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B191" s="2">
         <v>42947</v>
       </c>
@@ -12569,7 +12571,7 @@
         <v>32.049999999999997</v>
       </c>
     </row>
-    <row r="192" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B192" s="2">
         <v>42978</v>
       </c>
@@ -12625,7 +12627,7 @@
         <v>31.917000000000002</v>
       </c>
     </row>
-    <row r="193" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B193" s="2">
         <v>43008</v>
       </c>
@@ -12681,7 +12683,7 @@
         <v>32.064999999999998</v>
       </c>
     </row>
-    <row r="194" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B194" s="2">
         <v>43039</v>
       </c>
@@ -12737,7 +12739,7 @@
         <v>31.87</v>
       </c>
     </row>
-    <row r="195" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B195" s="2">
         <v>43069</v>
       </c>
@@ -12793,7 +12795,7 @@
         <v>31.611000000000001</v>
       </c>
     </row>
-    <row r="196" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B196" s="2">
         <v>43100</v>
       </c>
@@ -12849,7 +12851,7 @@
         <v>31.477</v>
       </c>
     </row>
-    <row r="197" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B197" s="2">
         <v>43131</v>
       </c>
@@ -12905,7 +12907,7 @@
         <v>31.756</v>
       </c>
     </row>
-    <row r="198" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B198" s="2">
         <v>43159</v>
       </c>
@@ -12961,7 +12963,7 @@
         <v>31.585999999999999</v>
       </c>
     </row>
-    <row r="199" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B199" s="2">
         <v>43190</v>
       </c>
@@ -13017,7 +13019,7 @@
         <v>31.408999999999999</v>
       </c>
     </row>
-    <row r="200" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B200" s="2">
         <v>43220</v>
       </c>
@@ -13073,7 +13075,7 @@
         <v>31.343</v>
       </c>
     </row>
-    <row r="201" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B201" s="2">
         <v>43251</v>
       </c>
@@ -13129,7 +13131,7 @@
         <v>31.228000000000002</v>
       </c>
     </row>
-    <row r="202" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B202" s="2">
         <v>43281</v>
       </c>
@@ -13185,7 +13187,7 @@
         <v>31.228999999999999</v>
       </c>
     </row>
-    <row r="203" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B203" s="2">
         <v>43312</v>
       </c>
@@ -13241,7 +13243,7 @@
         <v>31.286000000000001</v>
       </c>
     </row>
-    <row r="204" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B204" s="2">
         <v>43343</v>
       </c>
@@ -13297,7 +13299,7 @@
         <v>31.53</v>
       </c>
     </row>
-    <row r="205" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B205" s="2">
         <v>43373</v>
       </c>
@@ -13353,7 +13355,7 @@
         <v>31.666</v>
       </c>
     </row>
-    <row r="206" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B206" s="2">
         <v>43404</v>
       </c>
@@ -13409,7 +13411,7 @@
         <v>31.841000000000001</v>
       </c>
     </row>
-    <row r="207" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B207" s="2">
         <v>43434</v>
       </c>
@@ -13465,7 +13467,7 @@
         <v>31.596</v>
       </c>
     </row>
-    <row r="208" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B208" s="2">
         <v>43465</v>
       </c>
@@ -13521,7 +13523,7 @@
         <v>30.815999999999999</v>
       </c>
     </row>
-    <row r="209" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B209" s="2">
         <v>43496</v>
       </c>
@@ -13577,7 +13579,7 @@
         <v>30.155999999999999</v>
       </c>
     </row>
-    <row r="210" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B210" s="2">
         <v>43524</v>
       </c>
@@ -13633,7 +13635,7 @@
         <v>30.091000000000001</v>
       </c>
     </row>
-    <row r="211" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B211" s="2">
         <v>43555</v>
       </c>
@@ -13689,7 +13691,7 @@
         <v>29.594999999999999</v>
       </c>
     </row>
-    <row r="212" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B212" s="2">
         <v>43585</v>
       </c>
@@ -13745,7 +13747,7 @@
         <v>29.655000000000001</v>
       </c>
     </row>
-    <row r="213" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B213" s="2">
         <v>43616</v>
       </c>
@@ -13801,7 +13803,7 @@
         <v>29.335000000000001</v>
       </c>
     </row>
-    <row r="214" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B214" s="2">
         <v>43646</v>
       </c>
@@ -13857,7 +13859,7 @@
         <v>29.425000000000001</v>
       </c>
     </row>
-    <row r="215" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B215" s="2">
         <v>43677</v>
       </c>
@@ -13913,7 +13915,7 @@
         <v>29.004999999999999</v>
       </c>
     </row>
-    <row r="216" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B216" s="2">
         <v>43708</v>
       </c>
@@ -13969,7 +13971,7 @@
         <v>29.245000000000001</v>
       </c>
     </row>
-    <row r="217" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B217" s="2">
         <v>43738</v>
       </c>
@@ -14025,7 +14027,7 @@
         <v>27.684999999999999</v>
       </c>
     </row>
-    <row r="218" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B218" s="2">
         <v>43769</v>
       </c>
@@ -14081,7 +14083,7 @@
         <v>29.145</v>
       </c>
     </row>
-    <row r="219" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B219" s="2">
         <v>43799</v>
       </c>
@@ -14137,7 +14139,7 @@
         <v>29.004999999999999</v>
       </c>
     </row>
-    <row r="220" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B220" s="2">
         <v>43830</v>
       </c>
@@ -14193,7 +14195,7 @@
         <v>28.905000000000001</v>
       </c>
     </row>
-    <row r="221" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B221" s="2">
         <v>43861</v>
       </c>
@@ -14249,7 +14251,7 @@
         <v>28.67</v>
       </c>
     </row>
-    <row r="222" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B222" s="2">
         <v>43890</v>
       </c>
@@ -14305,7 +14307,7 @@
         <v>28.02</v>
       </c>
     </row>
-    <row r="223" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B223" s="2">
         <v>43921</v>
       </c>
@@ -14361,7 +14363,7 @@
         <v>28.14</v>
       </c>
     </row>
-    <row r="224" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B224" s="2">
         <v>43951</v>
       </c>
@@ -14417,7 +14419,7 @@
         <v>30.324999999999999</v>
       </c>
     </row>
-    <row r="225" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B225" s="2">
         <v>43982</v>
       </c>
@@ -14473,7 +14475,7 @@
         <v>24.28</v>
       </c>
     </row>
-    <row r="226" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B226" s="2">
         <v>44012</v>
       </c>
@@ -14529,7 +14531,7 @@
         <v>22.35</v>
       </c>
     </row>
-    <row r="227" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B227" s="2">
         <v>44043</v>
       </c>
@@ -14585,7 +14587,7 @@
         <v>22.975000000000001</v>
       </c>
     </row>
-    <row r="228" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B228" s="2">
         <v>44074</v>
       </c>
@@ -14641,7 +14643,7 @@
         <v>23.94</v>
       </c>
     </row>
-    <row r="229" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:43" x14ac:dyDescent="0.25">
       <c r="N229" s="2">
         <v>44104</v>
       </c>
@@ -14672,6 +14674,12 @@
       <c r="AE229">
         <v>55.9</v>
       </c>
+      <c r="AH229" s="2">
+        <v>44104</v>
+      </c>
+      <c r="AI229">
+        <v>0</v>
+      </c>
       <c r="AP229" s="2">
         <v>44104</v>
       </c>
@@ -14679,18 +14687,18 @@
         <v>24.015000000000001</v>
       </c>
     </row>
-    <row r="230" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:43" x14ac:dyDescent="0.25">
       <c r="N230" s="2">
         <v>44135</v>
       </c>
       <c r="O230">
-        <v>1350</v>
+        <v>1402</v>
       </c>
       <c r="R230" s="2">
         <v>44135</v>
       </c>
       <c r="S230">
-        <v>784</v>
+        <v>820</v>
       </c>
       <c r="AP230" s="2">
         <v>44135</v>
@@ -14699,7 +14707,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="231" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP231" s="2">
         <v>44165</v>
       </c>
@@ -14707,7 +14715,7 @@
         <v>25.79</v>
       </c>
     </row>
-    <row r="232" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP232" s="2">
         <v>44196</v>
       </c>
@@ -14715,7 +14723,7 @@
         <v>26.504999999999999</v>
       </c>
     </row>
-    <row r="233" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP233" s="2">
         <v>44227</v>
       </c>
@@ -14723,7 +14731,7 @@
         <v>27.56</v>
       </c>
     </row>
-    <row r="234" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP234" s="2">
         <v>44255</v>
       </c>
@@ -14731,7 +14739,7 @@
         <v>27.86</v>
       </c>
     </row>
-    <row r="235" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP235" s="2">
         <v>44286</v>
       </c>
@@ -14739,7 +14747,7 @@
         <v>27.96</v>
       </c>
     </row>
-    <row r="236" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP236" s="2">
         <v>44316</v>
       </c>
@@ -14747,7 +14755,7 @@
         <v>28.875</v>
       </c>
     </row>
-    <row r="237" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP237" s="2">
         <v>44347</v>
       </c>
@@ -14755,7 +14763,7 @@
         <v>28.961825999999999</v>
       </c>
     </row>
-    <row r="238" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP238" s="2">
         <v>44377</v>
       </c>
@@ -14763,7 +14771,7 @@
         <v>29.050485999999999</v>
       </c>
     </row>
-    <row r="239" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP239" s="2">
         <v>44408</v>
       </c>
@@ -14771,7 +14779,7 @@
         <v>29.099146000000001</v>
       </c>
     </row>
-    <row r="240" spans="2:43" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:43" x14ac:dyDescent="0.25">
       <c r="AP240" s="2">
         <v>44439</v>
       </c>
@@ -14779,7 +14787,7 @@
         <v>29.107806</v>
       </c>
     </row>
-    <row r="241" spans="42:43" x14ac:dyDescent="0.3">
+    <row r="241" spans="42:43" x14ac:dyDescent="0.25">
       <c r="AP241" s="2">
         <v>44469</v>
       </c>
@@ -14787,7 +14795,7 @@
         <v>29.116465000000002</v>
       </c>
     </row>
-    <row r="242" spans="42:43" x14ac:dyDescent="0.3">
+    <row r="242" spans="42:43" x14ac:dyDescent="0.25">
       <c r="AP242" s="2">
         <v>44500</v>
       </c>
@@ -14795,7 +14803,7 @@
         <v>29.125125000000001</v>
       </c>
     </row>
-    <row r="243" spans="42:43" x14ac:dyDescent="0.3">
+    <row r="243" spans="42:43" x14ac:dyDescent="0.25">
       <c r="AP243" s="2">
         <v>44530</v>
       </c>
@@ -14803,7 +14811,7 @@
         <v>29.133785</v>
       </c>
     </row>
-    <row r="244" spans="42:43" x14ac:dyDescent="0.3">
+    <row r="244" spans="42:43" x14ac:dyDescent="0.25">
       <c r="AP244" s="2">
         <v>44561</v>
       </c>

</xml_diff>